<commit_message>
got rid of template lines
allows whole program to run, even if nothing is actually being optimised (yet)
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\GitHub\MDOHPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D86F051-29AC-4931-B340-C701782E0F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E3AA3-CCCB-4D19-BAA5-FC1DC90B4827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>variable name</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>Pa</t>
+  </si>
+  <si>
+    <t>SFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific fuel consumption </t>
+  </si>
+  <si>
+    <t>kg/J</t>
+  </si>
+  <si>
+    <t>M_initial</t>
+  </si>
+  <si>
+    <t>initial guess of total mass</t>
   </si>
 </sst>
 </file>
@@ -204,12 +219,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +517,7 @@
     <col min="3" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -528,9 +542,8 @@
       <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -547,7 +560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -564,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -578,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -595,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -613,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -627,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -644,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -661,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -679,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -697,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -714,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -722,12 +735,47 @@
         <v>35</v>
       </c>
       <c r="C13">
-        <v>32200</v>
+        <f>88*C4+8*1550</f>
+        <v>32816</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
       </c>
       <c r="H13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>0.22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <v>240000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated pipe thermal study
now has real thermal study things in
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\GitHub\MDOHPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB14DB97-36A4-4C9C-B1FA-D1B46E22E0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF7DC57-D5DE-4CAB-BD0E-7F4A93E5B24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29880" yWindow="8880" windowWidth="15120" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
   <si>
     <t>variable name</t>
   </si>
@@ -215,18 +215,12 @@
     <t>specific heat capacity of LH2</t>
   </si>
   <si>
-    <t>J/gK</t>
-  </si>
-  <si>
     <t>LH2_max_T</t>
   </si>
   <si>
     <t>K</t>
   </si>
   <si>
-    <t>maximum allowed temperature of LH2 at 21psi</t>
-  </si>
-  <si>
     <t>LH2_T</t>
   </si>
   <si>
@@ -345,6 +339,60 @@
   </si>
   <si>
     <t>W/m^2</t>
+  </si>
+  <si>
+    <t>J/kg.K</t>
+  </si>
+  <si>
+    <t>maximum allowed temperature of LH2 at 21psi at the engine</t>
+  </si>
+  <si>
+    <t>L_H</t>
+  </si>
+  <si>
+    <t>latent heat of vaporisation of hydrogen</t>
+  </si>
+  <si>
+    <t>J/mol</t>
+  </si>
+  <si>
+    <t>mol_H</t>
+  </si>
+  <si>
+    <t>molar mass of hydrogen</t>
+  </si>
+  <si>
+    <t>kg/mol</t>
+  </si>
+  <si>
+    <t>boost_eta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boost pump efficiency </t>
+  </si>
+  <si>
+    <t>boost_m_eta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boost pump motor efficiency </t>
+  </si>
+  <si>
+    <t>boost_P</t>
+  </si>
+  <si>
+    <t>pressure rise from boost pump</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>boost_power_max</t>
+  </si>
+  <si>
+    <t>maximum power required in electric boost pump</t>
+  </si>
+  <si>
+    <t>hp</t>
   </si>
 </sst>
 </file>
@@ -467,8 +515,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE63AD13-E06B-4669-AFE2-130571A216A5}" name="Table1" displayName="Table1" ref="A1:H38" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A1:H38" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE63AD13-E06B-4669-AFE2-130571A216A5}" name="Table1" displayName="Table1" ref="A1:H44" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="A1:H44" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C839F816-2C44-4759-9D03-1220EC6D0D00}" name="variable name"/>
     <tableColumn id="2" xr3:uid="{2B325F69-EB23-449C-A232-3C0121C61395}" name="description"/>
@@ -746,10 +794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +1019,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>32816</v>
@@ -1062,7 +1110,7 @@
         <v>1.5049999999999999E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
@@ -1087,16 +1135,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20">
         <v>31.545909999999999</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -1104,17 +1152,17 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="5">
         <f>0.00000495/9.81</f>
         <v>5.0458715596330272E-7</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -1122,16 +1170,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
@@ -1139,16 +1187,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23">
         <v>2190</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
@@ -1156,17 +1204,17 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C24">
         <f>C14*C22*9.81/1000</f>
         <v>101.23920000000001</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -1174,17 +1222,17 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <f>C14/C23</f>
         <v>109.58904109589041</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -1192,17 +1240,17 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26">
         <f>5000/240</f>
         <v>20.833333333333332</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -1210,10 +1258,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27">
         <v>0.42199999999999999</v>
@@ -1275,16 +1323,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
         <v>57</v>
       </c>
       <c r="C31">
-        <v>4.2</v>
+        <v>12140</v>
       </c>
       <c r="D31" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="H31" t="b">
         <v>1</v>
@@ -1292,16 +1340,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
         <v>59</v>
-      </c>
-      <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32">
-        <v>21.5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>60</v>
       </c>
       <c r="H32" t="b">
         <v>1</v>
@@ -1309,16 +1357,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33">
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H33" t="b">
         <v>1</v>
@@ -1326,16 +1374,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34">
+        <v>0.04</v>
+      </c>
+      <c r="D34" t="s">
         <v>85</v>
-      </c>
-      <c r="B34" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34">
-        <v>0.09</v>
-      </c>
-      <c r="D34" t="s">
-        <v>87</v>
       </c>
       <c r="H34" t="b">
         <v>1</v>
@@ -1343,16 +1391,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C35">
         <v>0.34</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H35" t="b">
         <v>1</v>
@@ -1360,10 +1408,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36">
         <v>2.5399999999999999E-2</v>
@@ -1377,16 +1425,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37">
         <v>290</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H37" t="b">
         <v>1</v>
@@ -1394,18 +1442,115 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C38">
         <v>1.02E-4</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39">
+        <v>449.36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>104</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40">
+        <f>1.01*10^-3</f>
+        <v>1.01E-3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>107</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41">
+        <v>0.78</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42">
+        <v>0.86</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43">
+        <v>46</v>
+      </c>
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44">
+        <v>3.16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>117</v>
+      </c>
+      <c r="H44" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added struct and added formatting to constants
added constants and connections to struct after Tanika translated her functions to openMDAO syntax, currently contains 1 error in struct IDO and 1 in struct COG calcs

Co-Authored-By: tanikadodhia <124893487+tanikadodhia@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\GitHub\MDOHPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF7DC57-D5DE-4CAB-BD0E-7F4A93E5B24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB317C84-6916-4219-AF80-20D547C8B73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29880" yWindow="8880" windowWidth="15120" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="8880" windowWidth="15240" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="159">
   <si>
     <t>variable name</t>
   </si>
@@ -161,9 +161,6 @@
     <t>M_initial</t>
   </si>
   <si>
-    <t>initial guess of total mass</t>
-  </si>
-  <si>
     <t>LH2_rho</t>
   </si>
   <si>
@@ -393,6 +390,132 @@
   </si>
   <si>
     <t>hp</t>
+  </si>
+  <si>
+    <t>initial guess of total mass (from preliminary analysis)</t>
+  </si>
+  <si>
+    <t>Ka</t>
+  </si>
+  <si>
+    <t>bending moment constant 1</t>
+  </si>
+  <si>
+    <t>Ki</t>
+  </si>
+  <si>
+    <t>bending moment constant 2</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>youngs modulus</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>gravity</t>
+  </si>
+  <si>
+    <t>m/s^2</t>
+  </si>
+  <si>
+    <t>landing_acceleration</t>
+  </si>
+  <si>
+    <t>landing acceleration</t>
+  </si>
+  <si>
+    <t>tension_max</t>
+  </si>
+  <si>
+    <t>max tension landing gear</t>
+  </si>
+  <si>
+    <t>max_stress</t>
+  </si>
+  <si>
+    <t>wing stress max</t>
+  </si>
+  <si>
+    <t>max_deflection</t>
+  </si>
+  <si>
+    <t>wing deflections max</t>
+  </si>
+  <si>
+    <t>thic_chord_rat</t>
+  </si>
+  <si>
+    <t>thickness to chord ratio for wing root</t>
+  </si>
+  <si>
+    <t>tail_hc</t>
+  </si>
+  <si>
+    <t>horizontal tail chord</t>
+  </si>
+  <si>
+    <t>tail_hs</t>
+  </si>
+  <si>
+    <t>horizontal tail span</t>
+  </si>
+  <si>
+    <t>tail_h_angle</t>
+  </si>
+  <si>
+    <t>average tail angle</t>
+  </si>
+  <si>
+    <t>tail_vc</t>
+  </si>
+  <si>
+    <t>vertical tail chord</t>
+  </si>
+  <si>
+    <t>tail_vh</t>
+  </si>
+  <si>
+    <t>vertical tail height</t>
+  </si>
+  <si>
+    <t>tail_v_angle</t>
+  </si>
+  <si>
+    <t>average tail angle vertical</t>
+  </si>
+  <si>
+    <t>root_taper_chord_ratio</t>
+  </si>
+  <si>
+    <t>tail taper chord ratio</t>
+  </si>
+  <si>
+    <t>constant_uht</t>
+  </si>
+  <si>
+    <t>tail constant</t>
+  </si>
+  <si>
+    <t>fuselage_diameter</t>
+  </si>
+  <si>
+    <t>fuselage diameter</t>
+  </si>
+  <si>
+    <t>fuselage_taper</t>
+  </si>
+  <si>
+    <t>taper of fuselage</t>
+  </si>
+  <si>
+    <t>f_wet_area</t>
+  </si>
+  <si>
+    <t>fuselage wetted area</t>
   </si>
 </sst>
 </file>
@@ -475,7 +598,54 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
@@ -515,8 +685,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE63AD13-E06B-4669-AFE2-130571A216A5}" name="Table1" displayName="Table1" ref="A1:H44" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
-  <autoFilter ref="A1:H44" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE63AD13-E06B-4669-AFE2-130571A216A5}" name="Table1" displayName="Table1" ref="A1:H64" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5">
+  <autoFilter ref="A1:H64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C839F816-2C44-4759-9D03-1220EC6D0D00}" name="variable name"/>
     <tableColumn id="2" xr3:uid="{2B325F69-EB23-449C-A232-3C0121C61395}" name="description"/>
@@ -794,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,9 +1016,6 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -863,6 +1030,9 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
@@ -877,8 +1047,8 @@
       <c r="C4">
         <v>232</v>
       </c>
-      <c r="H4" t="b">
-        <v>0</v>
+      <c r="F4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -894,8 +1064,8 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" t="b">
-        <v>0</v>
+      <c r="F5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -911,6 +1081,9 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" t="b">
         <v>1</v>
       </c>
@@ -925,8 +1098,8 @@
       <c r="C7">
         <v>0.7</v>
       </c>
-      <c r="H7" t="b">
-        <v>0</v>
+      <c r="F7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -942,9 +1115,6 @@
       <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -959,9 +1129,6 @@
       <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -976,9 +1143,6 @@
       <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -993,8 +1157,8 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
-      <c r="H11" t="b">
-        <v>0</v>
+      <c r="F11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1010,22 +1174,22 @@
       <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>32816</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
@@ -1036,7 +1200,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="C14">
         <v>240000</v>
@@ -1044,16 +1208,19 @@
       <c r="D14" t="s">
         <v>36</v>
       </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
       </c>
       <c r="C15">
         <v>69.295869999999994</v>
@@ -1067,10 +1234,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
       </c>
       <c r="C16">
         <v>2823.3503000000001</v>
@@ -1084,10 +1251,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
       </c>
       <c r="C17">
         <v>49.657200000000003</v>
@@ -1101,16 +1268,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
       </c>
       <c r="C18">
         <v>1.5049999999999999E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
@@ -1118,10 +1285,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" t="s">
-        <v>50</v>
       </c>
       <c r="C19">
         <v>5.0000000000000001E-3</v>
@@ -1135,16 +1302,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
         <v>97</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
       </c>
       <c r="C20">
         <v>31.545909999999999</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -1152,17 +1319,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="5">
+        <v>5.0458715596330272E-7</v>
+      </c>
+      <c r="D21" t="s">
         <v>64</v>
-      </c>
-      <c r="C21" s="5">
-        <f>0.00000495/9.81</f>
-        <v>5.0458715596330272E-7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -1170,16 +1336,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
         <v>66</v>
-      </c>
-      <c r="B22" t="s">
-        <v>67</v>
       </c>
       <c r="C22">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
@@ -1187,16 +1353,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
         <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>70</v>
       </c>
       <c r="C23">
         <v>2190</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
@@ -1204,17 +1370,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
         <v>72</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24">
+        <v>101.23920000000001</v>
+      </c>
+      <c r="D24" t="s">
         <v>73</v>
-      </c>
-      <c r="C24">
-        <f>C14*C22*9.81/1000</f>
-        <v>101.23920000000001</v>
-      </c>
-      <c r="D24" t="s">
-        <v>74</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -1222,35 +1387,33 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
         <v>75</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25">
+        <v>109.58904109589041</v>
+      </c>
+      <c r="D25" t="s">
         <v>76</v>
       </c>
-      <c r="C25">
-        <f>C14/C23</f>
-        <v>109.58904109589041</v>
-      </c>
-      <c r="D25" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" t="b">
-        <v>0</v>
+      <c r="F25" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
         <v>78</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26">
+        <v>20.833333333333332</v>
+      </c>
+      <c r="D26" t="s">
         <v>79</v>
-      </c>
-      <c r="C26">
-        <f>5000/240</f>
-        <v>20.833333333333332</v>
-      </c>
-      <c r="D26" t="s">
-        <v>80</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -1258,10 +1421,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
         <v>81</v>
-      </c>
-      <c r="B27" t="s">
-        <v>82</v>
       </c>
       <c r="C27">
         <v>0.42199999999999999</v>
@@ -1272,10 +1435,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
         <v>51</v>
-      </c>
-      <c r="B28" t="s">
-        <v>52</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -1283,16 +1446,19 @@
       <c r="D28" t="s">
         <v>6</v>
       </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
       <c r="H28" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29">
         <v>40</v>
@@ -1300,16 +1466,19 @@
       <c r="D29" t="s">
         <v>6</v>
       </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
       <c r="H29" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -1317,22 +1486,25 @@
       <c r="D30" t="s">
         <v>6</v>
       </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
       <c r="H30" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31">
         <v>12140</v>
       </c>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H31" t="b">
         <v>1</v>
@@ -1340,16 +1512,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32">
         <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H32" t="b">
         <v>1</v>
@@ -1357,16 +1529,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
         <v>60</v>
-      </c>
-      <c r="B33" t="s">
-        <v>61</v>
       </c>
       <c r="C33">
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H33" t="b">
         <v>1</v>
@@ -1374,16 +1546,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
         <v>83</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
       </c>
       <c r="C34">
         <v>0.04</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H34" t="b">
         <v>1</v>
@@ -1391,16 +1563,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" t="s">
         <v>86</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
       </c>
       <c r="C35">
         <v>0.34</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H35" t="b">
         <v>1</v>
@@ -1408,10 +1580,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
         <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>89</v>
       </c>
       <c r="C36">
         <v>2.5399999999999999E-2</v>
@@ -1425,16 +1597,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" t="s">
         <v>90</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
       </c>
       <c r="C37">
         <v>290</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H37" t="b">
         <v>1</v>
@@ -1442,16 +1614,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
         <v>92</v>
-      </c>
-      <c r="B38" t="s">
-        <v>93</v>
       </c>
       <c r="C38">
         <v>1.02E-4</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H38" t="b">
         <v>1</v>
@@ -1459,16 +1631,16 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
         <v>102</v>
-      </c>
-      <c r="B39" t="s">
-        <v>103</v>
       </c>
       <c r="C39">
         <v>449.36</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H39" t="b">
         <v>1</v>
@@ -1476,17 +1648,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" t="s">
         <v>105</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40">
+        <v>1.01E-3</v>
+      </c>
+      <c r="D40" t="s">
         <v>106</v>
-      </c>
-      <c r="C40">
-        <f>1.01*10^-3</f>
-        <v>1.01E-3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>107</v>
       </c>
       <c r="H40" t="b">
         <v>1</v>
@@ -1494,10 +1665,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" t="s">
         <v>108</v>
-      </c>
-      <c r="B41" t="s">
-        <v>109</v>
       </c>
       <c r="C41">
         <v>0.78</v>
@@ -1508,10 +1679,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" t="s">
         <v>110</v>
-      </c>
-      <c r="B42" t="s">
-        <v>111</v>
       </c>
       <c r="C42">
         <v>0.86</v>
@@ -1522,16 +1693,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
         <v>112</v>
-      </c>
-      <c r="B43" t="s">
-        <v>113</v>
       </c>
       <c r="C43">
         <v>46</v>
       </c>
       <c r="D43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H43" t="b">
         <v>1</v>
@@ -1539,23 +1710,367 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" t="s">
         <v>115</v>
-      </c>
-      <c r="B44" t="s">
-        <v>116</v>
       </c>
       <c r="C44">
         <v>3.16</v>
       </c>
       <c r="D44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45">
+        <v>0.6</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47">
+        <v>90000000</v>
+      </c>
+      <c r="D47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48">
+        <v>9.81</v>
+      </c>
+      <c r="D48" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50">
+        <v>9000000</v>
+      </c>
+      <c r="D50" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>131</v>
+      </c>
+      <c r="B51" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51">
+        <v>10000000</v>
+      </c>
+      <c r="D51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53">
+        <v>0.127</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54">
+        <v>5.5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55">
+        <v>16</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56">
+        <v>30</v>
+      </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>147</v>
+      </c>
+      <c r="B59" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59">
+        <v>32.5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>149</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60">
+        <v>0.09</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63">
+        <v>0.12</v>
+      </c>
+      <c r="F63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64">
+        <v>442</v>
+      </c>
+      <c r="D64" t="s">
+        <v>76</v>
+      </c>
+      <c r="F64" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="E2:H2">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:H64">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(E2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
small fixes to systems and MDO part
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\GitHub\MDOHPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84B4801-D6DC-4958-9A1E-C6EAB2A46849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A80057A-FEED-47A4-9989-9819F8BB8640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29640" yWindow="-5640" windowWidth="15480" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,7 +937,7 @@
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="B34" sqref="B33:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,6 +1151,9 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1398,6 +1401,9 @@
       <c r="F25" t="b">
         <v>1</v>
       </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1784,6 +1790,9 @@
         <v>126</v>
       </c>
       <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed fuel mass eq and connected some variables
also added solver in correct way, now gets proper convergence but no optimisation (no desvars)
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\GitHub\MDOHPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A80057A-FEED-47A4-9989-9819F8BB8640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2CA111-309E-4BA8-B5AC-A1F06106BDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="-5640" windowWidth="15480" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="8880" windowWidth="15240" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="156">
   <si>
     <t>variable name</t>
   </si>
@@ -254,21 +254,9 @@
     <t>N/m^2</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>thrust</t>
-  </si>
-  <si>
-    <t>kN</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>wing area</t>
-  </si>
-  <si>
     <t>m^2</t>
   </si>
   <si>
@@ -516,6 +504,9 @@
   </si>
   <si>
     <t>fuselage wetted area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wing area INITIAL </t>
   </si>
 </sst>
 </file>
@@ -655,8 +646,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE63AD13-E06B-4669-AFE2-130571A216A5}" name="Table1" displayName="Table1" ref="A1:H64" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
-  <autoFilter ref="A1:H64" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE63AD13-E06B-4669-AFE2-130571A216A5}" name="Table1" displayName="Table1" ref="A1:H63" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
+  <autoFilter ref="A1:H63" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C839F816-2C44-4759-9D03-1220EC6D0D00}" name="variable name"/>
     <tableColumn id="2" xr3:uid="{2B325F69-EB23-449C-A232-3C0121C61395}" name="description"/>
@@ -934,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B33:C34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1185,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C14">
         <v>240000</v>
@@ -1274,7 +1265,7 @@
         <v>1.5049999999999999E-2</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
@@ -1299,16 +1290,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C20">
         <v>31.545909999999999</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
@@ -1322,7 +1313,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="5">
-        <v>5.0458715596330272E-7</v>
+        <v>6.0639E-5</v>
       </c>
       <c r="D21" t="s">
         <v>64</v>
@@ -1370,13 +1361,19 @@
         <v>71</v>
       </c>
       <c r="B24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24">
+        <v>109.58904109589041</v>
+      </c>
+      <c r="D24" t="s">
         <v>72</v>
       </c>
-      <c r="C24">
-        <v>101.23920000000001</v>
-      </c>
-      <c r="D24" t="s">
-        <v>73</v>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
       </c>
       <c r="H24" t="b">
         <v>1</v>
@@ -1384,22 +1381,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
         <v>74</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25">
+        <v>20.833333333333332</v>
+      </c>
+      <c r="D25" t="s">
         <v>75</v>
-      </c>
-      <c r="C25">
-        <v>109.58904109589041</v>
-      </c>
-      <c r="D25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
@@ -1407,16 +1398,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
       <c r="C26">
-        <v>20.833333333333332</v>
-      </c>
-      <c r="D26" t="s">
-        <v>79</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
@@ -1424,13 +1412,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C27">
-        <v>0.42199999999999999</v>
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
       </c>
       <c r="H27" t="b">
         <v>1</v>
@@ -1438,13 +1432,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -1458,13 +1452,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1478,19 +1472,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>12140</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="H30" t="b">
         <v>1</v>
@@ -1498,16 +1489,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="C31">
-        <v>12140</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="H31" t="b">
         <v>1</v>
@@ -1515,13 +1506,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C32">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D32" t="s">
         <v>58</v>
@@ -1532,16 +1523,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C33">
-        <v>20</v>
+        <v>0.04</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="H33" t="b">
         <v>1</v>
@@ -1549,16 +1540,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
         <v>82</v>
       </c>
-      <c r="B34" t="s">
-        <v>83</v>
-      </c>
       <c r="C34">
-        <v>0.04</v>
+        <v>0.34</v>
       </c>
       <c r="D34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H34" t="b">
         <v>1</v>
@@ -1566,16 +1557,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C35">
-        <v>0.34</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="H35" t="b">
         <v>1</v>
@@ -1583,16 +1574,19 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C36">
-        <v>2.5399999999999999E-2</v>
+        <v>290</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>58</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
       </c>
       <c r="H36" t="b">
         <v>1</v>
@@ -1600,19 +1594,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37">
+        <v>1.02E-4</v>
+      </c>
+      <c r="D37" t="s">
         <v>89</v>
-      </c>
-      <c r="B37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37">
-        <v>290</v>
-      </c>
-      <c r="D37" t="s">
-        <v>58</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
       </c>
       <c r="H37" t="b">
         <v>1</v>
@@ -1620,16 +1611,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C38">
-        <v>1.02E-4</v>
+        <v>449.36</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="H38" t="b">
         <v>1</v>
@@ -1637,16 +1628,16 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" t="s">
         <v>101</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39">
+        <v>1.01E-3</v>
+      </c>
+      <c r="D39" t="s">
         <v>102</v>
-      </c>
-      <c r="C39">
-        <v>449.36</v>
-      </c>
-      <c r="D39" t="s">
-        <v>103</v>
       </c>
       <c r="H39" t="b">
         <v>1</v>
@@ -1654,16 +1645,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" t="s">
         <v>104</v>
       </c>
-      <c r="B40" t="s">
-        <v>105</v>
-      </c>
       <c r="C40">
-        <v>1.01E-3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>106</v>
+        <v>0.78</v>
       </c>
       <c r="H40" t="b">
         <v>1</v>
@@ -1671,13 +1659,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C41">
-        <v>0.78</v>
+        <v>0.86</v>
       </c>
       <c r="H41" t="b">
         <v>1</v>
@@ -1685,13 +1673,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
         <v>109</v>
-      </c>
-      <c r="B42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C42">
-        <v>0.86</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
@@ -1699,16 +1690,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" t="s">
         <v>111</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43">
+        <v>3.16</v>
+      </c>
+      <c r="D43" t="s">
         <v>112</v>
-      </c>
-      <c r="C43">
-        <v>46</v>
-      </c>
-      <c r="D43" t="s">
-        <v>113</v>
       </c>
       <c r="H43" t="b">
         <v>1</v>
@@ -1722,24 +1713,21 @@
         <v>115</v>
       </c>
       <c r="C44">
-        <v>3.16</v>
-      </c>
-      <c r="D44" t="s">
-        <v>116</v>
-      </c>
-      <c r="H44" t="b">
+        <v>0.6</v>
+      </c>
+      <c r="F44" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C45">
-        <v>0.6</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -1747,13 +1735,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C46">
-        <v>3.5999999999999997E-2</v>
+        <v>90000000</v>
+      </c>
+      <c r="D46" t="s">
+        <v>38</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -1761,53 +1752,53 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47">
+        <v>9.81</v>
+      </c>
+      <c r="D47" t="s">
         <v>122</v>
       </c>
-      <c r="B47" t="s">
-        <v>123</v>
-      </c>
-      <c r="C47">
-        <v>90000000</v>
-      </c>
-      <c r="D47" t="s">
-        <v>38</v>
-      </c>
       <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
         <v>124</v>
       </c>
-      <c r="B48" t="s">
-        <v>125</v>
-      </c>
       <c r="C48">
-        <v>9.81</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F48" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>9000000</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
@@ -1815,13 +1806,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C50">
-        <v>9000000</v>
+        <v>10000000</v>
       </c>
       <c r="D50" t="s">
         <v>38</v>
@@ -1832,16 +1823,16 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C51">
-        <v>10000000</v>
+        <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -1849,16 +1840,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B52" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C52">
-        <v>3</v>
-      </c>
-      <c r="D52" t="s">
-        <v>6</v>
+        <v>0.127</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
@@ -1866,27 +1854,33 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C53">
-        <v>0.127</v>
+        <v>5.5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
       </c>
       <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C54">
-        <v>5.5</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -1894,22 +1888,19 @@
       <c r="F54" t="b">
         <v>1</v>
       </c>
-      <c r="H54" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C55">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -1917,16 +1908,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C56">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
@@ -1934,10 +1925,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -1951,13 +1942,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C58">
-        <v>6</v>
+        <v>32.5</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
@@ -1968,13 +1959,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B59" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C59">
-        <v>32.5</v>
+        <v>0.09</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
@@ -1985,16 +1976,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B60" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C60">
-        <v>0.09</v>
-      </c>
-      <c r="D60" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F60" t="b">
         <v>1</v>
@@ -2002,72 +1990,58 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
       </c>
       <c r="F61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C62">
-        <v>7</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6</v>
+        <v>0.12</v>
       </c>
       <c r="F62" t="b">
-        <v>1</v>
-      </c>
-      <c r="H62" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B63" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C63">
-        <v>0.12</v>
+        <v>442</v>
+      </c>
+      <c r="D63" t="s">
+        <v>72</v>
       </c>
       <c r="F63" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>157</v>
-      </c>
-      <c r="B64" t="s">
-        <v>158</v>
-      </c>
-      <c r="C64">
-        <v>442</v>
-      </c>
-      <c r="D64" t="s">
-        <v>76</v>
-      </c>
-      <c r="F64" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E2:H64">
+  <conditionalFormatting sqref="E2:H63">
     <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(E2))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
lil changes and connections
</commit_message>
<xml_diff>
--- a/constants.xlsx
+++ b/constants.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\Year 4\MECH5080M Team Project\7 - MDOHPCA\MDOHPCA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\GitHub\MDOHPCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3CA14A-621E-4700-A912-54536B20F8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555D7926-1B31-4F8A-A919-20D8070B129A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29640" yWindow="-5640" windowWidth="15480" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,13 +549,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -579,13 +592,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,18 +943,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -965,7 +980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -982,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1008,7 +1023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1022,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1059,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1096,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1113,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -1133,7 +1148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1159,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1173,7 +1188,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1193,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1216,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1233,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1250,7 +1265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1267,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1284,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1301,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1318,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1335,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1352,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1369,7 +1384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -1392,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1409,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1423,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1443,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1463,7 +1478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1483,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -1500,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1517,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1534,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -1551,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -1568,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -1585,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -1605,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -1622,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -1639,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>99</v>
       </c>
@@ -1656,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>102</v>
       </c>
@@ -1670,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -1684,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -1701,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -1718,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -1732,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -1746,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -1763,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>119</v>
       </c>
@@ -1783,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>122</v>
       </c>
@@ -1800,15 +1815,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>124</v>
       </c>
       <c r="B49" t="s">
         <v>125</v>
       </c>
-      <c r="C49">
-        <v>9000000</v>
+      <c r="C49" s="7">
+        <v>90000000</v>
       </c>
       <c r="D49" t="s">
         <v>37</v>
@@ -1817,15 +1832,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>126</v>
       </c>
       <c r="B50" t="s">
         <v>127</v>
       </c>
-      <c r="C50">
-        <v>10000000</v>
+      <c r="C50" s="6">
+        <v>1140000000</v>
       </c>
       <c r="D50" t="s">
         <v>37</v>
@@ -1834,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>128</v>
       </c>
@@ -1851,7 +1866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -1865,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>132</v>
       </c>
@@ -1885,7 +1900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>134</v>
       </c>
@@ -1902,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>136</v>
       </c>
@@ -1919,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>138</v>
       </c>
@@ -1936,7 +1951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>140</v>
       </c>
@@ -1953,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -1970,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>144</v>
       </c>
@@ -1987,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>146</v>
       </c>
@@ -2001,7 +2016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -2021,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>150</v>
       </c>
@@ -2035,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>152</v>
       </c>
@@ -2052,7 +2067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>156</v>
       </c>
@@ -2066,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>158</v>
       </c>

</xml_diff>